<commit_message>
Cleanup results and add them as pdf
</commit_message>
<xml_diff>
--- a/Studie1/Pretask-Answers_Studie1.xlsx
+++ b/Studie1/Pretask-Answers_Studie1.xlsx
@@ -5,20 +5,29 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael_M\Documents\GitHub\BA_Analyse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael_M\Documents\GitHub\BA_Analyse\Studie1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B13FCF-399E-4468-8201-E933780C7FA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FDD8CDD-A10D-490A-8AD3-ABE5DAB5553B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Antworten" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -472,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D316B3B-172B-4D03-A326-485829F85AAB}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -488,7 +497,7 @@
     <col min="6" max="6" width="36.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="100.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.90625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="58.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="16" width="21.54296875" style="1" customWidth="1"/>
     <col min="17" max="16384" width="14.453125" style="1"/>
@@ -782,6 +791,18 @@
         <v>0</v>
       </c>
     </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I11" s="1">
+        <f>AVERAGE(I2:I9)</f>
+        <v>24.75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I12" s="1">
+        <f>STDEVA(I2:I9)</f>
+        <v>3.6936238496708271</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>